<commit_message>
Importacion de modulos de transacciones
</commit_message>
<xml_diff>
--- a/Archivo_Importacion_TransaccionEquipos.xlsx
+++ b/Archivo_Importacion_TransaccionEquipos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12510" tabRatio="500"/>
+    <workbookView windowWidth="28800" windowHeight="12495" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -145,11 +145,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -178,7 +178,44 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -189,11 +226,41 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -205,8 +272,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -221,48 +295,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -276,42 +311,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -348,187 +348,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -557,6 +557,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -568,24 +586,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -620,6 +620,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -637,15 +646,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -657,138 +657,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -810,54 +810,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="Título 3" xfId="1" builtinId="18"/>
+    <cellStyle name="Moneda [0]" xfId="2" builtinId="7"/>
+    <cellStyle name="40% - Énfasis1" xfId="3" builtinId="31"/>
+    <cellStyle name="Coma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Moneda" xfId="5" builtinId="4"/>
+    <cellStyle name="Coma" xfId="6" builtinId="3"/>
+    <cellStyle name="Porcentaje" xfId="7" builtinId="5"/>
+    <cellStyle name="Hipervínculo" xfId="8" builtinId="8"/>
+    <cellStyle name="Hipervínculo visitado" xfId="9" builtinId="9"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21"/>
+    <cellStyle name="Nota" xfId="11" builtinId="10"/>
+    <cellStyle name="Título 2" xfId="12" builtinId="17"/>
+    <cellStyle name="Texto de advertencia" xfId="13" builtinId="11"/>
+    <cellStyle name="Título" xfId="14" builtinId="15"/>
+    <cellStyle name="Texto explicativo" xfId="15" builtinId="53"/>
+    <cellStyle name="Título 1" xfId="16" builtinId="16"/>
+    <cellStyle name="Título 4" xfId="17" builtinId="19"/>
+    <cellStyle name="Entrada" xfId="18" builtinId="20"/>
+    <cellStyle name="Cálculo" xfId="19" builtinId="22"/>
+    <cellStyle name="Celda de comprobación" xfId="20" builtinId="23"/>
+    <cellStyle name="Celda vinculada" xfId="21" builtinId="24"/>
+    <cellStyle name="Total" xfId="22" builtinId="25"/>
+    <cellStyle name="Correcto" xfId="23" builtinId="26"/>
+    <cellStyle name="40% - Énfasis5" xfId="24" builtinId="47"/>
+    <cellStyle name="Incorrecto" xfId="25" builtinId="27"/>
+    <cellStyle name="Neutro" xfId="26" builtinId="28"/>
+    <cellStyle name="20% - Énfasis5" xfId="27" builtinId="46"/>
+    <cellStyle name="Énfasis1" xfId="28" builtinId="29"/>
+    <cellStyle name="20% - Énfasis1" xfId="29" builtinId="30"/>
+    <cellStyle name="60% - Énfasis1" xfId="30" builtinId="32"/>
+    <cellStyle name="20% - Énfasis6" xfId="31" builtinId="50"/>
+    <cellStyle name="Énfasis2" xfId="32" builtinId="33"/>
+    <cellStyle name="20% - Énfasis2" xfId="33" builtinId="34"/>
+    <cellStyle name="40% - Énfasis2" xfId="34" builtinId="35"/>
+    <cellStyle name="60% - Énfasis2" xfId="35" builtinId="36"/>
+    <cellStyle name="Énfasis3" xfId="36" builtinId="37"/>
+    <cellStyle name="20% - Énfasis3" xfId="37" builtinId="38"/>
+    <cellStyle name="40% - Énfasis3" xfId="38" builtinId="39"/>
+    <cellStyle name="60% - Énfasis3" xfId="39" builtinId="40"/>
+    <cellStyle name="Énfasis4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Énfasis4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Énfasis4" xfId="42" builtinId="43"/>
+    <cellStyle name="60% - Énfasis4" xfId="43" builtinId="44"/>
+    <cellStyle name="Énfasis5" xfId="44" builtinId="45"/>
+    <cellStyle name="60% - Énfasis5" xfId="45" builtinId="48"/>
+    <cellStyle name="Énfasis6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Énfasis6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Énfasis6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1196,8 +1196,8 @@
   <sheetPr/>
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23:K28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>

</xml_diff>